<commit_message>
Update OWASP_penetration testing checklist.xlsx
</commit_message>
<xml_diff>
--- a/OWASP_penetration testing checklist.xlsx
+++ b/OWASP_penetration testing checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E676467-2758-4E18-9B35-7B06AD5C1951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B01480-B7E8-438E-9A0D-B3AAD685020C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -738,9 +738,6 @@
     <t>Test Local Storage</t>
   </si>
   <si>
-    <t>Use a search engine to search for Network diagrams and Configurations, Credentials, Error message content.</t>
-  </si>
-  <si>
     <t>Find the version and type of a running web server to determine known vulnerabilities and the appropriate exploits. Using
 "HTTP header field ordering" and "Malformed requests test".</t>
   </si>
@@ -752,9 +749,6 @@
   </si>
   <si>
     <t>Find applications hosted in the webserver (Virtual hosts/Subdomain), non-standard ports, DNS zone transfers</t>
-  </si>
-  <si>
-    <t>Google Hacking, Sitedigger, Shodan, FOCA, Punkspider</t>
   </si>
   <si>
     <t>Find sensitive information from webpage comments and Metadata on source code.</t>
@@ -1235,6 +1229,13 @@
   </si>
   <si>
     <t>Penetration testing checklist</t>
+  </si>
+  <si>
+    <t>Use a search engine to search for Network diagrams and Configurations, Credentials, Error message content.
+(Exp: google hacking: site:example.com ; site:example.com ext:pdf  ; "index of/" site:example.com ;</t>
+  </si>
+  <si>
+    <t>Google Hacking, Shodan.io, FOCA, Punkspider</t>
   </si>
 </sst>
 </file>
@@ -3362,7 +3363,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B1" s="31"/>
       <c r="E1" s="11"/>
@@ -3397,7 +3398,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="46.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -3405,10 +3406,10 @@
         <v>42</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>226</v>
+        <v>369</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>231</v>
+        <v>370</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>29</v>
@@ -3422,10 +3423,10 @@
         <v>43</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>227</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>228</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>29</v>
@@ -3439,10 +3440,10 @@
         <v>44</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>29</v>
@@ -3456,10 +3457,10 @@
         <v>45</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>29</v>
@@ -3473,10 +3474,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>29</v>
@@ -3493,7 +3494,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>29</v>
@@ -3507,10 +3508,10 @@
         <v>47</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>29</v>
@@ -3524,10 +3525,10 @@
         <v>48</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>29</v>
@@ -3542,10 +3543,10 @@
         <v>49</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>29</v>
@@ -3560,10 +3561,10 @@
         <v>50</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>29</v>
@@ -3605,10 +3606,10 @@
         <v>59</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>29</v>
@@ -3622,10 +3623,10 @@
         <v>60</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>29</v>
@@ -3642,7 +3643,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>29</v>
@@ -3659,7 +3660,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>29</v>
@@ -3676,7 +3677,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>29</v>
@@ -3690,10 +3691,10 @@
         <v>64</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>29</v>
@@ -3707,10 +3708,10 @@
         <v>65</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>29</v>
@@ -3725,10 +3726,10 @@
         <v>66</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>29</v>
@@ -3769,10 +3770,10 @@
         <v>75</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>29</v>
@@ -3786,10 +3787,10 @@
         <v>76</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>29</v>
@@ -3804,10 +3805,10 @@
         <v>77</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>29</v>
@@ -3825,7 +3826,7 @@
         <v>15</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>29</v>
@@ -3840,10 +3841,10 @@
         <v>79</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>29</v>
@@ -3858,10 +3859,10 @@
         <v>80</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>29</v>
@@ -3876,10 +3877,10 @@
         <v>81</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>29</v>
@@ -3921,10 +3922,10 @@
         <v>92</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>29</v>
@@ -3938,10 +3939,10 @@
         <v>93</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>29</v>
@@ -3955,10 +3956,10 @@
         <v>94</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>29</v>
@@ -3972,10 +3973,10 @@
         <v>95</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>29</v>
@@ -3989,10 +3990,10 @@
         <v>96</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>29</v>
@@ -4006,10 +4007,10 @@
         <v>97</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>29</v>
@@ -4023,10 +4024,10 @@
         <v>98</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>29</v>
@@ -4041,10 +4042,10 @@
         <v>99</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>29</v>
@@ -4058,10 +4059,10 @@
         <v>100</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>29</v>
@@ -4075,10 +4076,10 @@
         <v>101</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>29</v>
@@ -4119,10 +4120,10 @@
         <v>106</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>29</v>
@@ -4136,10 +4137,10 @@
         <v>107</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>29</v>
@@ -4156,7 +4157,7 @@
         <v>16</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>29</v>
@@ -4170,10 +4171,10 @@
         <v>109</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>29</v>
@@ -4216,10 +4217,10 @@
         <v>119</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>29</v>
@@ -4233,10 +4234,10 @@
         <v>120</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>29</v>
@@ -4250,10 +4251,10 @@
         <v>121</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>29</v>
@@ -4268,10 +4269,10 @@
         <v>122</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>29</v>
@@ -4285,10 +4286,10 @@
         <v>123</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>29</v>
@@ -4302,10 +4303,10 @@
         <v>124</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>29</v>
@@ -4319,10 +4320,10 @@
         <v>125</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>29</v>
@@ -4336,10 +4337,10 @@
         <v>126</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>29</v>
@@ -4382,10 +4383,10 @@
         <v>127</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>29</v>
@@ -4399,10 +4400,10 @@
         <v>128</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>29</v>
@@ -4416,10 +4417,10 @@
         <v>129</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>29</v>
@@ -4434,10 +4435,10 @@
         <v>130</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>29</v>
@@ -4451,10 +4452,10 @@
         <v>131</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>29</v>
@@ -4466,10 +4467,10 @@
         <v>132</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>29</v>
@@ -4481,10 +4482,10 @@
         <v>133</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>29</v>
@@ -4496,10 +4497,10 @@
         <v>134</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>29</v>
@@ -4510,10 +4511,10 @@
         <v>135</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>29</v>
@@ -4526,10 +4527,10 @@
         <v>136</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>29</v>
@@ -4541,10 +4542,10 @@
         <v>137</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>29</v>
@@ -4558,10 +4559,10 @@
         <v>138</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>29</v>
@@ -4578,7 +4579,7 @@
         <v>19</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>29</v>
@@ -4592,10 +4593,10 @@
         <v>140</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>29</v>
@@ -4609,10 +4610,10 @@
         <v>141</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>29</v>
@@ -4626,10 +4627,10 @@
         <v>142</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>29</v>
@@ -4643,10 +4644,10 @@
         <v>143</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>29</v>
@@ -4660,10 +4661,10 @@
         <v>144</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>29</v>
@@ -4675,10 +4676,10 @@
         <v>145</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D82" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>29</v>
@@ -4691,10 +4692,10 @@
         <v>146</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>29</v>
@@ -4709,10 +4710,10 @@
         <v>147</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>29</v>
@@ -4730,7 +4731,7 @@
         <v>20</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>29</v>
@@ -4781,10 +4782,10 @@
         <v>152</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D89" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>29</v>
@@ -4802,7 +4803,7 @@
         <v>21</v>
       </c>
       <c r="D90" s="27" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>29</v>
@@ -4844,10 +4845,10 @@
         <v>171</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>29</v>
@@ -4862,10 +4863,10 @@
         <v>172</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>29</v>
@@ -4907,10 +4908,10 @@
         <v>176</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>29</v>
@@ -4925,10 +4926,10 @@
         <v>177</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>29</v>
@@ -4943,10 +4944,10 @@
         <v>178</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E99" s="20" t="s">
         <v>29</v>
@@ -4987,10 +4988,10 @@
         <v>192</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E102" s="20" t="s">
         <v>29</v>
@@ -5004,10 +5005,10 @@
         <v>193</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E103" s="20" t="s">
         <v>29</v>
@@ -5021,10 +5022,10 @@
         <v>194</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E104" s="20" t="s">
         <v>29</v>
@@ -5039,10 +5040,10 @@
         <v>195</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E105" s="20" t="s">
         <v>29</v>
@@ -5057,10 +5058,10 @@
         <v>196</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E106" s="20" t="s">
         <v>29</v>
@@ -5075,10 +5076,10 @@
         <v>197</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E107" s="20" t="s">
         <v>29</v>
@@ -5093,10 +5094,10 @@
         <v>198</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E108" s="20" t="s">
         <v>29</v>
@@ -5111,10 +5112,10 @@
         <v>199</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E109" s="20" t="s">
         <v>29</v>
@@ -5129,10 +5130,10 @@
         <v>200</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E110" s="20" t="s">
         <v>29</v>
@@ -5178,7 +5179,7 @@
         <v>17</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E113" s="20" t="s">
         <v>29</v>
@@ -5193,10 +5194,10 @@
         <v>215</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E114" s="20" t="s">
         <v>29</v>
@@ -5211,10 +5212,10 @@
         <v>216</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D115" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E115" s="20" t="s">
         <v>29</v>
@@ -5229,10 +5230,10 @@
         <v>217</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E116" s="20" t="s">
         <v>29</v>
@@ -5247,10 +5248,10 @@
         <v>218</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E117" s="20" t="s">
         <v>29</v>
@@ -5265,10 +5266,10 @@
         <v>219</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E118" s="20" t="s">
         <v>29</v>
@@ -5283,10 +5284,10 @@
         <v>220</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E119" s="20" t="s">
         <v>29</v>
@@ -5304,7 +5305,7 @@
         <v>18</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E120" s="20" t="s">
         <v>29</v>
@@ -5319,10 +5320,10 @@
         <v>222</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E121" s="20" t="s">
         <v>29</v>
@@ -5337,10 +5338,10 @@
         <v>223</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D122" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E122" s="20" t="s">
         <v>29</v>
@@ -5354,10 +5355,10 @@
         <v>224</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D123" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E123" s="20" t="s">
         <v>29</v>
@@ -5372,10 +5373,10 @@
         <v>225</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E124" s="20" t="s">
         <v>29</v>
@@ -5993,16 +5994,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>8</v>
@@ -6014,13 +6015,13 @@
         <v>27</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
@@ -6028,13 +6029,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>158</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>26</v>
@@ -6048,7 +6049,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>